<commit_message>
Extent Report Integration with REST API Cucumber Framework
</commit_message>
<xml_diff>
--- a/CORE_API_TestData.xlsx
+++ b/CORE_API_TestData.xlsx
@@ -111,13 +111,13 @@
     <t>TC009</t>
   </si>
   <si>
-    <t>test.rest144@test.com</t>
-  </si>
-  <si>
-    <t>test.rest145@test.com</t>
-  </si>
-  <si>
-    <t>test.rest146@test.com</t>
+    <t>test.rest147@test.com</t>
+  </si>
+  <si>
+    <t>test.rest148@test.com</t>
+  </si>
+  <si>
+    <t>test.rest150@test.com</t>
   </si>
 </sst>
 </file>
@@ -836,7 +836,7 @@
     <hyperlink ref="B6" r:id="rId5"/>
     <hyperlink ref="B7" r:id="rId6"/>
     <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9:B11" r:id="rId8" display="test.rest144@test.com"/>
+    <hyperlink ref="B9:B11" r:id="rId8" display="test.rest147@test.com"/>
     <hyperlink ref="B9" r:id="rId9"/>
     <hyperlink ref="B11" r:id="rId10"/>
   </hyperlinks>

</xml_diff>